<commit_message>
coding and mcq handled
</commit_message>
<xml_diff>
--- a/testcontents/TestContentReport.xlsx
+++ b/testcontents/TestContentReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="53">
   <si>
     <t>Question Type</t>
   </si>
@@ -52,6 +52,9 @@
     <t>10</t>
   </si>
   <si>
+    <t xml:space="preserve">a b d e </t>
+  </si>
+  <si>
     <t>Subjective</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t>20</t>
   </si>
   <si>
+    <t xml:space="preserve">C C++ Java JavaScript Python 3 </t>
+  </si>
+  <si>
     <t>MQ</t>
   </si>
   <si>
@@ -145,16 +151,25 @@
     <t>hajkds</t>
   </si>
   <si>
+    <t xml:space="preserve">a b </t>
+  </si>
+  <si>
     <t>mcqabc@</t>
   </si>
   <si>
     <t>ghajkld;f</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;script&gt;alert("Hello! This is a JavaScript alert.");&lt;/script&gt; dfghj </t>
+  </si>
+  <si>
     <t>coding 1</t>
   </si>
   <si>
     <t>jksjfhksajdfhkas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java </t>
   </si>
   <si>
     <t>coding 1 Clone</t>
@@ -202,7 +217,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -236,58 +251,148 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>22</v>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -297,7 +402,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -331,58 +436,165 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>26</v>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -426,44 +638,53 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>